<commit_message>
made kr2 suggested changes, ready for more ;)
</commit_message>
<xml_diff>
--- a/t/TestData/sampleValidation/test-meta.xlsx
+++ b/t/TestData/sampleValidation/test-meta.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Tissue_ID</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>test_sample.1.bam</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>test_sample.2.bam</t>
   </si>
 </sst>
 </file>
@@ -383,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,6 +447,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated test dataset to allow is_normal_for_donor column in input
</commit_message>
<xml_diff>
--- a/t/TestData/sampleValidation/test-meta.xlsx
+++ b/t/TestData/sampleValidation/test-meta.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx2/nfs_link/2016_11_28_Pan Prostate/cgpNgsQc/t/TestData/sampleValidation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx2/nfs_link/2016_11_28_Pan_Prostate/cgpNgsQc/t/TestData/sampleValidation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5540" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="7040" yWindow="460" windowWidth="24480" windowHeight="17680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test-meta" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Tissue_ID</t>
   </si>
@@ -65,31 +65,38 @@
     <t>test_sample.1.bam</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>test 2</t>
   </si>
   <si>
     <t>test_sample.2.bam</t>
+  </si>
+  <si>
+    <t>is_normal_for_donor</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>test_sample.3.bam</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>test-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Courier"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,9 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,22 +398,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -418,16 +426,19 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -437,17 +448,17 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -455,13 +466,36 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>